<commit_message>
changes made created Journal Entries for the Financial Year 2022-2023
</commit_message>
<xml_diff>
--- a/JournalEntriesForReceivable.xlsx
+++ b/JournalEntriesForReceivable.xlsx
@@ -15,15 +15,14 @@
     <sheet name="OCTOBER_2022" r:id="rId9" sheetId="7"/>
     <sheet name="NOVEMBER_2022" r:id="rId10" sheetId="8"/>
     <sheet name="DECEMBER_2022" r:id="rId11" sheetId="9"/>
-    <sheet name="JANUARY_2023" r:id="rId12" sheetId="10"/>
-    <sheet name="FEBRUARY_2023" r:id="rId13" sheetId="11"/>
-    <sheet name="MARCH_2023" r:id="rId14" sheetId="12"/>
+    <sheet name="FEBRUARY_2023" r:id="rId12" sheetId="10"/>
+    <sheet name="MARCH_2023" r:id="rId13" sheetId="11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5002" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4996" uniqueCount="553">
   <si>
     <t>Date</t>
   </si>
@@ -8999,39 +8998,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9103,7 +9069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F19"/>
   <sheetViews>

</xml_diff>